<commit_message>
Capture Screenshot in Extent Reports - commits
</commit_message>
<xml_diff>
--- a/src/test/resources/testcases/Testcases.xlsx
+++ b/src/test/resources/testcases/Testcases.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB82D8D1-F7CE-4B31-B005-748A0042DEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E47119B-EA47-4397-B4B1-D809DCAE6FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="CarePlan Suite" sheetId="2" r:id="rId2"/>
-    <sheet name="CarePlan Suite_old" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="TestCases" sheetId="5" r:id="rId1"/>
+    <sheet name="dummyTest" sheetId="1" r:id="rId2"/>
+    <sheet name="CarePlan Suite" sheetId="2" r:id="rId3"/>
+    <sheet name="CarePlan Suite_old" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="107">
   <si>
     <t>TCID</t>
   </si>
@@ -858,12 +859,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1941B540-9AFD-417B-8571-ACF26D5F52FA}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1682,11 +1683,695 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="35.1796875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="39.08984375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="15">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="16">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="16">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="16">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="16">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="16">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1715,7 +2400,7 @@
         <v>79</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>78</v>
@@ -1989,7 +2674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FD8452-C0EF-48E4-B465-8B8A8AAC04C2}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -2264,7 +2949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Sample commits for Demo
</commit_message>
<xml_diff>
--- a/src/test/resources/testcases/Testcases.xlsx
+++ b/src/test/resources/testcases/Testcases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D47E05C-89FB-4E5A-A5A5-5A4AB2404453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A802D2E3-8916-4514-BF0C-FB5855BB6688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="110">
   <si>
     <t>TCID</t>
   </si>
@@ -347,10 +347,19 @@
     <t>XXXXXXX</t>
   </si>
   <si>
-    <t xml:space="preserve">Christine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amelia </t>
+    <t>facility</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>.//h1[contains(text(),'oldString')]</t>
+  </si>
+  <si>
+    <t>Orli</t>
+  </si>
+  <si>
+    <t>Grimes</t>
   </si>
 </sst>
 </file>
@@ -505,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -556,6 +565,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,14 +872,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1941B540-9AFD-417B-8571-ACF26D5F52FA}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
     <col min="2" max="2" width="13" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="15.54296875" customWidth="1"/>
     <col min="4" max="4" width="28.453125" style="9" customWidth="1"/>
@@ -1020,15 +1030,17 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="10"/>
+        <v>107</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -1250,13 +1262,13 @@
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
@@ -1268,13 +1280,13 @@
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="26" t="s">
         <v>44</v>
       </c>
       <c r="G22" s="3"/>
@@ -1288,13 +1300,13 @@
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
@@ -1306,13 +1318,13 @@
       <c r="C24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="26" t="s">
         <v>48</v>
       </c>
       <c r="G24" s="4"/>
@@ -1326,13 +1338,13 @@
       <c r="C25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="12"/>
+      <c r="F25" s="10"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
@@ -1344,13 +1356,13 @@
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="26" t="s">
         <v>47</v>
       </c>
       <c r="G26" s="3"/>
@@ -1364,13 +1376,13 @@
       <c r="C27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="12"/>
+      <c r="F27" s="10"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
@@ -1382,13 +1394,13 @@
       <c r="C28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="26" t="s">
         <v>53</v>
       </c>
       <c r="G28" s="3"/>
@@ -1402,13 +1414,13 @@
       <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="26" t="s">
         <v>59</v>
       </c>
       <c r="G29" s="3"/>
@@ -1422,13 +1434,13 @@
       <c r="C30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="26" t="s">
         <v>60</v>
       </c>
       <c r="G30" s="3"/>
@@ -1442,13 +1454,13 @@
       <c r="C31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="2"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
@@ -1460,13 +1472,13 @@
       <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="26" t="s">
         <v>61</v>
       </c>
       <c r="G32" s="3"/>
@@ -1480,13 +1492,13 @@
       <c r="C33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="26" t="s">
         <v>67</v>
       </c>
       <c r="G33" s="3"/>
@@ -1500,13 +1512,13 @@
       <c r="C34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F34" s="12"/>
+      <c r="F34" s="10"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
@@ -1521,7 +1533,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="2"/>
       <c r="F35" s="16">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -1684,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1716,7 +1728,7 @@
         <v>79</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>78</v>
@@ -1772,217 +1784,232 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>106</v>
       </c>
       <c r="D5" s="18"/>
-      <c r="E5" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>92</v>
-      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="22" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="22" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="B15" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="C15" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>101</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:G14 B14:C14" xr:uid="{D448F840-58E2-4284-9E6E-F1E0F9B4092C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15:G15 B15:C15" xr:uid="{D448F840-58E2-4284-9E6E-F1E0F9B4092C}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>